<commit_message>
Lab5 and lab6 are finished
</commit_message>
<xml_diff>
--- a/Lab4/levels_of_testing_Alexander_Kovalyov.xlsx
+++ b/Lab4/levels_of_testing_Alexander_Kovalyov.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
   </bookViews>
   <sheets>
     <sheet name="Components tests" sheetId="1" r:id="rId1"/>
@@ -594,7 +594,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B37"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection sqref="A1:B37"/>
     </sheetView>
   </sheetViews>
@@ -909,7 +909,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>

</xml_diff>